<commit_message>
Working and paralled thread
</commit_message>
<xml_diff>
--- a/Adani-BUWise-Websites.xlsx
+++ b/Adani-BUWise-Websites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python-Projects\Health\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB3934B-18EC-4A84-960B-029781DA1F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB346E7-D517-4643-9084-218189016BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26535" yWindow="-360" windowWidth="21600" windowHeight="11235" xr2:uid="{27A08A2E-3D32-40C2-A803-D2E0912A5285}"/>
+    <workbookView xWindow="-28920" yWindow="-2745" windowWidth="29040" windowHeight="15720" xr2:uid="{27A08A2E-3D32-40C2-A803-D2E0912A5285}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>S. No</t>
   </si>
@@ -66,17 +66,6 @@
   </si>
   <si>
     <t>Airports</t>
-  </si>
-  <si>
-    <t>www.adaniairports.com
-svpia-ahmedabad.adaniairports.com
-www.adani.com/ccsia-lucknow-airport
-www.adani.com/mangaluru-airport
-csmia-mumbai.adaniairports.com
-www.adani.com/jaipur-airport
-www.adani.com/lgbia-guwahati-airport
-thiruvananthapuram.adaniairports.com
-navimumbai.adaniairports.com</t>
   </si>
   <si>
     <t>Green Energy</t>
@@ -222,7 +211,6 @@
   </si>
   <si>
     <t>www.bprpl.in
-uat-s.crfindia.org
 www.avrpl.com
 www.bkrpl.com
 www.kkrpl.com
@@ -231,6 +219,23 @@
 www.skrpl.com
 www.vbppl.in
 www.ksrpl.co.in</t>
+  </si>
+  <si>
+    <t>https://drpmumbai.maharashtra.gov.in/</t>
+  </si>
+  <si>
+    <t>DRP</t>
+  </si>
+  <si>
+    <t>www.adaniairports.com
+svpia-ahmedabad.adaniairports.com
+www.adani.com/ccsia-lucknow-airport
+mangaluru.adaniairports.com/
+csmia-mumbai.adaniairports.com
+www.adani.com/jaipur-airport
+www.adani.com/lgbia-guwahati-airport
+thiruvananthapuram.adaniairports.com
+navimumbai.adaniairports.com</t>
   </si>
 </sst>
 </file>
@@ -935,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CF85520-8546-440F-926E-0527E8D9D1E0}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -963,7 +968,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="162" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="145.80000000000001" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -971,10 +976,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="64.8" x14ac:dyDescent="0.3">
@@ -988,7 +993,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="81" x14ac:dyDescent="0.3">
@@ -999,10 +1004,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="145.80000000000001" x14ac:dyDescent="0.3">
@@ -1013,10 +1018,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="81" x14ac:dyDescent="0.3">
@@ -1024,13 +1029,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
@@ -1038,13 +1043,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="64.8" x14ac:dyDescent="0.3">
@@ -1052,13 +1057,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1066,13 +1071,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="275.39999999999998" x14ac:dyDescent="0.3">
@@ -1080,13 +1085,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="32.4" x14ac:dyDescent="0.3">
@@ -1094,13 +1099,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -1108,13 +1113,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="D12" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="48.6" x14ac:dyDescent="0.3">
@@ -1122,13 +1127,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
@@ -1136,13 +1141,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>25</v>
-      </c>
       <c r="D14" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
@@ -1150,13 +1155,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="D15" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1164,13 +1169,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>33</v>
-      </c>
       <c r="D16" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
@@ -1178,13 +1183,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="D17" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1192,13 +1197,27 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1210,10 +1229,11 @@
     <hyperlink ref="C11" r:id="rId5" xr:uid="{FAD1BE04-1766-440B-9182-1A554208FA7D}"/>
     <hyperlink ref="C16" r:id="rId6" display="www.adanibunkering.com" xr:uid="{B2831486-2AC9-416E-A52C-32ED7BEC7D9A}"/>
     <hyperlink ref="C18" r:id="rId7" display="www.areprl.com" xr:uid="{7ACABEF8-BFED-42FB-BF03-425CBE872FCE}"/>
+    <hyperlink ref="C19" r:id="rId8" xr:uid="{DF4648E7-4DE9-48D4-AF4A-D4C66BEE056A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>